<commit_message>
character assets and min/max character count
</commit_message>
<xml_diff>
--- a/Burndown.xlsx
+++ b/Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c4e25a7e6f3dc489/Documents/GitHub/ConcurrentProgrammingGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="312" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5F17C0A-C343-40ED-A2ED-98AE3AEDCF05}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12790F0E-9465-4139-BA52-AA6854EAA655}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2834,6 +2834,9 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -6827,7 +6830,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7311,6 +7314,9 @@
       <c r="C37">
         <v>6</v>
       </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
       <c r="G37" s="9" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Pause Menu, Character Objects, Play Pause Step Fast Forward and Stop Game
</commit_message>
<xml_diff>
--- a/Burndown.xlsx
+++ b/Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c4e25a7e6f3dc489/Documents/GitHub/ConcurrentProgrammingGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12790F0E-9465-4139-BA52-AA6854EAA655}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A50FF1E7-0823-4DA4-958E-78BAB196EE20}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1113,6 +1113,18 @@
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2838,6 +2850,18 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6829,8 +6853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7202,6 +7226,9 @@
       <c r="C28">
         <v>2</v>
       </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
@@ -7213,6 +7240,9 @@
       <c r="C29">
         <v>2</v>
       </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
@@ -7224,6 +7254,9 @@
       <c r="C30">
         <v>1</v>
       </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
@@ -7235,6 +7268,9 @@
       <c r="C31">
         <v>0</v>
       </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
@@ -7266,7 +7302,7 @@
       <c r="D34">
         <v>7</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -7300,7 +7336,7 @@
       <c r="D36">
         <v>5</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -7331,6 +7367,9 @@
       <c r="C38">
         <v>5</v>
       </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
       <c r="G38" s="9" t="s">
         <v>33</v>
       </c>
@@ -7345,7 +7384,10 @@
       <c r="C39">
         <v>5</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -7359,6 +7401,9 @@
       <c r="C40">
         <v>4</v>
       </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
       <c r="G40" s="2" t="s">
         <v>35</v>
       </c>
@@ -7372,6 +7417,9 @@
       </c>
       <c r="C41">
         <v>4</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Character Death, Health Bars, Skirmish Customization
</commit_message>
<xml_diff>
--- a/Burndown.xlsx
+++ b/Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c4e25a7e6f3dc489/Documents/GitHub/ConcurrentProgrammingGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="733" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4F1F39B-7B82-4A0B-877D-069936656985}"/>
+  <xr:revisionPtr revIDLastSave="901" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69D4AC07-EE3B-4F4E-B5D5-4AB1C358C2A6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
   <si>
     <t>Times</t>
   </si>
@@ -183,13 +183,31 @@
     <t>Sprint 4 Backlog:</t>
   </si>
   <si>
-    <t>Battle functionality</t>
-  </si>
-  <si>
     <t>Create Skirmish Battle</t>
   </si>
   <si>
     <t>Customise Skirmish Battle</t>
+  </si>
+  <si>
+    <t>Battle Model</t>
+  </si>
+  <si>
+    <t>Rescheduling</t>
+  </si>
+  <si>
+    <t>Message passing</t>
+  </si>
+  <si>
+    <t>Yielding</t>
+  </si>
+  <si>
+    <t>Character Death</t>
+  </si>
+  <si>
+    <t>End Game Victory / Defeat</t>
+  </si>
+  <si>
+    <t>Health Bars</t>
   </si>
 </sst>
 </file>
@@ -299,10 +317,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,6 +845,614 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Analysis</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> of the Effects of Maximum Queue Time on Processor Performance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.3875745974306118E-2"/>
+          <c:y val="1.291793854112736E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SchedulerAnalysis!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Wait Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SchedulerAnalysis!$E$3:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SchedulerAnalysis!$F$3:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.7826675999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1718307000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5130024000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8956689999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.2616687000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.6101710000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.9606605000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.3139970000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.6245069999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.8903300000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.2603349999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D3F6-4384-809A-B76B7708CAD5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1193815088"/>
+        <c:axId val="1193808432"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SchedulerAnalysis!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Processor Steps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SchedulerAnalysis!$E$3:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SchedulerAnalysis!$G$3:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>251.56268</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>251.74047999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>251.83994999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>252.06460000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>252.18398999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>252.25443000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>252.44098</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>252.63681</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>252.81992</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>252.94544999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>253.11206000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D3F6-4384-809A-B76B7708CAD5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1633873728"/>
+        <c:axId val="1601814368"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1193815088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1193808432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1193808432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="25400" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1193815088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1601814368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1633873728"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1633873728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1601814368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.5354330708661411E-2"/>
+          <c:y val="0.90335593467483233"/>
+          <c:w val="0.91540223097112872"/>
+          <c:h val="7.8125546806649182E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1367,7 +1993,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3534,7 +4160,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3933,7 +4559,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4465,40 +5091,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
@@ -4688,6 +5314,547 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Sprint 4 Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Burndown!$C$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planned</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Burndown!$B$52:$B$65</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>44995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Burndown!$C$52:$C$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-29A3-4E6B-9986-4FEF1C02DC2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Burndown!$D$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Burndown!$B$52:$B$65</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>44995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Burndown!$D$52:$D$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-29A3-4E6B-9986-4FEF1C02DC2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="129552912"/>
+        <c:axId val="178301920"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="129552912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="178301920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="178301920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="129552912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5264,614 +6431,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Analysis</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> of the Effects of Maximum Queue Time on Processor Performance</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="9.3875745974306118E-2"/>
-          <c:y val="1.291793854112736E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>SchedulerAnalysis!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Average Wait Time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>SchedulerAnalysis!$E$3:$E$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>SchedulerAnalysis!$F$3:$F$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>5.7826675999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.1718307000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.5130024000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.8956689999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.2616687000000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.6101710000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.9606605000000004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.3139970000000005</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.6245069999999995</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.8903300000000005</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.2603349999999995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D3F6-4384-809A-B76B7708CAD5}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1193815088"/>
-        <c:axId val="1193808432"/>
-      </c:lineChart>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>SchedulerAnalysis!$G$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Average Processor Steps</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>SchedulerAnalysis!$E$3:$E$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>SchedulerAnalysis!$G$3:$G$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>251.56268</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>251.74047999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>251.83994999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>252.06460000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>252.18398999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>252.25443000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>252.44098</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>252.63681</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>252.81992</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>252.94544999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>253.11206000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D3F6-4384-809A-B76B7708CAD5}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1633873728"/>
-        <c:axId val="1601814368"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1193815088"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1193808432"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1193808432"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="25400" cmpd="sng">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1193815088"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1601814368"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1633873728"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="1633873728"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1601814368"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="3.5354330708661411E-2"/>
-          <c:y val="0.90335593467483233"/>
-          <c:w val="0.91540223097112872"/>
-          <c:h val="7.8125546806649182E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5953,6 +6512,46 @@
 </file>
 
 <file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7847,8 +8446,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -7956,6 +8555,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -7966,6 +8570,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -7997,6 +8606,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8350,7 +8962,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8853,7 +9465,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9356,7 +9968,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9859,7 +10471,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10362,7 +10974,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10865,8 +11477,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -10974,11 +11586,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -10989,11 +11596,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -11025,9 +11627,509 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -12146,6 +13248,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>97971</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>402771</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>65315</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A215D3A4-9DC5-C86F-359B-D7744C4F1729}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -12600,10 +13738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12611,9 +13749,10 @@
     <col min="2" max="2" width="23.5546875" customWidth="1"/>
     <col min="5" max="5" width="10.109375" customWidth="1"/>
     <col min="7" max="7" width="41.88671875" customWidth="1"/>
+    <col min="27" max="27" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -12630,7 +13769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -12647,7 +13786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -12663,8 +13802,9 @@
       <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="AA3" s="8"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -12680,8 +13820,9 @@
       <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="AA4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -12697,8 +13838,9 @@
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AA5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -12714,8 +13856,9 @@
       <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="AA6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -12731,8 +13874,9 @@
       <c r="G7" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="AA7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -12748,8 +13892,9 @@
       <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="AA8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -12765,13 +13910,30 @@
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="AA9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="G10" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="AA10" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA11" s="8"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA12" s="8"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA13" s="8"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA14" s="8"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA15" s="8"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -12787,8 +13949,9 @@
       <c r="G16" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="AA16" s="8"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -12804,8 +13967,9 @@
       <c r="G17" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="AA17" s="8"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -12821,8 +13985,9 @@
       <c r="G18" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="AA18" s="8"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -12838,8 +14003,9 @@
       <c r="G19" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="AA19" s="8"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -12855,8 +14021,9 @@
       <c r="G20" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="AA20" s="8"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
@@ -12872,8 +14039,9 @@
       <c r="G21" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="AA21" s="8"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -12889,8 +14057,9 @@
       <c r="G22" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="AA22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
@@ -12904,8 +14073,9 @@
         <v>1</v>
       </c>
       <c r="G23" s="6"/>
+      <c r="AA23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
@@ -12919,8 +14089,9 @@
         <v>1</v>
       </c>
       <c r="G24" s="6"/>
+      <c r="AA24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -12934,8 +14105,9 @@
         <v>1</v>
       </c>
       <c r="G25" s="6"/>
+      <c r="AA25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -12949,8 +14121,9 @@
         <v>1</v>
       </c>
       <c r="G26" s="6"/>
+      <c r="AA26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>5</v>
       </c>
@@ -12964,8 +14137,9 @@
         <v>0</v>
       </c>
       <c r="G27" s="6"/>
+      <c r="AA27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>6</v>
       </c>
@@ -12978,8 +14152,9 @@
       <c r="D28">
         <v>0</v>
       </c>
+      <c r="AA28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -12992,8 +14167,9 @@
       <c r="D29">
         <v>0</v>
       </c>
+      <c r="AA29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>1</v>
       </c>
@@ -13006,8 +14182,9 @@
       <c r="D30">
         <v>0</v>
       </c>
+      <c r="AA30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
@@ -13020,8 +14197,12 @@
       <c r="D31">
         <v>0</v>
       </c>
+      <c r="AA31" s="8"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA32" s="8"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>0</v>
       </c>
@@ -13037,8 +14218,9 @@
       <c r="G33" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="AA33" s="8"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -13054,8 +14236,9 @@
       <c r="G34" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="AA34" s="8"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>3</v>
       </c>
@@ -13071,8 +14254,9 @@
       <c r="G35" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="AA35" s="8"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>4</v>
       </c>
@@ -13088,8 +14272,9 @@
       <c r="G36" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="AA36" s="8"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>5</v>
       </c>
@@ -13105,8 +14290,9 @@
       <c r="G37" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="AA37" s="8"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>6</v>
       </c>
@@ -13122,8 +14308,9 @@
       <c r="G38" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="AA38" s="8"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -13139,8 +14326,9 @@
       <c r="G39" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="AA39" s="8"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>1</v>
       </c>
@@ -13156,8 +14344,9 @@
       <c r="G40" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="AA40" s="8"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>2</v>
       </c>
@@ -13170,8 +14359,9 @@
       <c r="D41">
         <v>2</v>
       </c>
+      <c r="AA41" s="8"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>3</v>
       </c>
@@ -13184,8 +14374,9 @@
       <c r="D42">
         <v>2</v>
       </c>
+      <c r="AA42" s="8"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>4</v>
       </c>
@@ -13198,8 +14389,9 @@
       <c r="D43">
         <v>1</v>
       </c>
+      <c r="AA43" s="8"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>5</v>
       </c>
@@ -13212,8 +14404,9 @@
       <c r="D44">
         <v>1</v>
       </c>
+      <c r="AA44" s="8"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>6</v>
       </c>
@@ -13226,8 +14419,9 @@
       <c r="D45">
         <v>1</v>
       </c>
+      <c r="AA45" s="8"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -13240,8 +14434,9 @@
       <c r="D46">
         <v>1</v>
       </c>
+      <c r="AA46" s="8"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>1</v>
       </c>
@@ -13249,17 +14444,25 @@
         <v>44994</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
+      <c r="AA47" s="8"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="9"/>
+      <c r="AA48" s="8"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA49" s="8"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA50" s="8"/>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -13275,8 +14478,9 @@
       <c r="G51" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="AA51" s="8"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -13284,16 +14488,17 @@
         <v>44995</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D52">
-        <v>3</v>
-      </c>
-      <c r="G52" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="AA52" s="8"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -13301,13 +14506,16 @@
         <v>44996</v>
       </c>
       <c r="C53">
-        <v>3</v>
-      </c>
-      <c r="G53" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53">
+        <v>8</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>4</v>
       </c>
@@ -13315,13 +14523,16 @@
         <v>44997</v>
       </c>
       <c r="C54">
-        <v>3</v>
-      </c>
-      <c r="G54" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54">
+        <v>7</v>
+      </c>
+      <c r="G54" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>5</v>
       </c>
@@ -13329,11 +14540,16 @@
         <v>44998</v>
       </c>
       <c r="C55">
-        <v>3</v>
-      </c>
-      <c r="G55" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>6</v>
       </c>
@@ -13341,11 +14557,13 @@
         <v>44999</v>
       </c>
       <c r="C56">
-        <v>3</v>
-      </c>
-      <c r="G56" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>7</v>
       </c>
@@ -13353,11 +14571,13 @@
         <v>45000</v>
       </c>
       <c r="C57">
-        <v>3</v>
-      </c>
-      <c r="G57" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>1</v>
       </c>
@@ -13365,10 +14585,13 @@
         <v>45001</v>
       </c>
       <c r="C58">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>2</v>
       </c>
@@ -13376,10 +14599,13 @@
         <v>45002</v>
       </c>
       <c r="C59">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G59" s="14" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>3</v>
       </c>
@@ -13387,10 +14613,13 @@
         <v>45003</v>
       </c>
       <c r="C60">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>4</v>
       </c>
@@ -13398,10 +14627,10 @@
         <v>45004</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>5</v>
       </c>
@@ -13409,10 +14638,10 @@
         <v>45005</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>6</v>
       </c>
@@ -13420,10 +14649,10 @@
         <v>45006</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>7</v>
       </c>
@@ -13482,23 +14711,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
       <c r="R1" s="10"/>

</xml_diff>

<commit_message>
some animations, text on damage and player bases
</commit_message>
<xml_diff>
--- a/Burndown.xlsx
+++ b/Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c4e25a7e6f3dc489/Documents/GitHub/ConcurrentProgrammingGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="901" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69D4AC07-EE3B-4F4E-B5D5-4AB1C358C2A6}"/>
+  <xr:revisionPtr revIDLastSave="905" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AB9CDA5-170A-4B1C-93CA-91BC1E28D4C7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5641,6 +5641,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13741,7 +13747,7 @@
   <dimension ref="A1:AA65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14545,7 +14551,7 @@
       <c r="D55">
         <v>5</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="G55" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -14559,6 +14565,9 @@
       <c r="C56">
         <v>7</v>
       </c>
+      <c r="D56">
+        <v>5</v>
+      </c>
       <c r="G56" s="14" t="s">
         <v>52</v>
       </c>
@@ -14573,6 +14582,9 @@
       <c r="C57">
         <v>6</v>
       </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
       <c r="G57" s="14" t="s">
         <v>53</v>
       </c>
@@ -14615,7 +14627,7 @@
       <c r="C60">
         <v>4</v>
       </c>
-      <c r="G60" s="14" t="s">
+      <c r="G60" s="2" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Background overhaul, message passing, yielding, game over
</commit_message>
<xml_diff>
--- a/Burndown.xlsx
+++ b/Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c4e25a7e6f3dc489/Documents/GitHub/ConcurrentProgrammingGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="905" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AB9CDA5-170A-4B1C-93CA-91BC1E28D4C7}"/>
+  <xr:revisionPtr revIDLastSave="1000" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F00DFBDC-84E1-4FA8-B6B0-5D053FC82FC3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="59">
   <si>
     <t>Times</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>Health Bars</t>
+  </si>
+  <si>
+    <t>Locking</t>
+  </si>
+  <si>
+    <t>Charging</t>
   </si>
 </sst>
 </file>
@@ -5014,6 +5020,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -5029,6 +5036,7 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -5091,22 +5099,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>6</c:v>
@@ -5115,7 +5123,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4</c:v>
@@ -5328,31 +5336,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Sprint 4 Burndown Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5407,6 +5390,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -5484,22 +5468,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>6</c:v>
@@ -5508,7 +5492,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4</c:v>
@@ -5531,7 +5515,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-29A3-4E6B-9986-4FEF1C02DC2A}"/>
+              <c16:uniqueId val="{00000000-A5F2-4351-9950-04FD164E32E8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5631,22 +5615,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5654,7 +5653,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-29A3-4E6B-9986-4FEF1C02DC2A}"/>
+              <c16:uniqueId val="{00000001-A5F2-4351-9950-04FD164E32E8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5668,11 +5667,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="129552912"/>
-        <c:axId val="178301920"/>
+        <c:axId val="1003459487"/>
+        <c:axId val="1003435359"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="129552912"/>
+        <c:axId val="1003459487"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5715,14 +5714,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178301920"/>
+        <c:crossAx val="1003435359"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="178301920"/>
+        <c:axId val="1003435359"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5773,7 +5772,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129552912"/>
+        <c:crossAx val="1003459487"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5791,7 +5790,10 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -13262,22 +13264,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>97971</xdr:colOff>
+      <xdr:colOff>32657</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>97972</xdr:rowOff>
+      <xdr:rowOff>54428</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>402771</xdr:colOff>
+      <xdr:colOff>337457</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>65315</xdr:rowOff>
+      <xdr:rowOff>21771</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9">
+        <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A215D3A4-9DC5-C86F-359B-D7744C4F1729}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D4ECB38-BB0A-C8EE-2F7A-18D16D9DFCC3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13747,7 +13749,7 @@
   <dimension ref="A1:AA65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14494,10 +14496,10 @@
         <v>44995</v>
       </c>
       <c r="C52">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D52">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>48</v>
@@ -14512,10 +14514,10 @@
         <v>44996</v>
       </c>
       <c r="C53">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D53">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>49</v>
@@ -14529,12 +14531,12 @@
         <v>44997</v>
       </c>
       <c r="C54">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D54">
-        <v>7</v>
-      </c>
-      <c r="G54" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -14546,10 +14548,10 @@
         <v>44998</v>
       </c>
       <c r="C55">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>51</v>
@@ -14563,12 +14565,12 @@
         <v>44999</v>
       </c>
       <c r="C56">
+        <v>8</v>
+      </c>
+      <c r="D56">
         <v>7</v>
       </c>
-      <c r="D56">
-        <v>5</v>
-      </c>
-      <c r="G56" s="14" t="s">
+      <c r="G56" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -14580,13 +14582,13 @@
         <v>45000</v>
       </c>
       <c r="C57">
+        <v>7</v>
+      </c>
+      <c r="D57">
         <v>6</v>
       </c>
-      <c r="D57">
-        <v>4</v>
-      </c>
       <c r="G57" s="14" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.3">
@@ -14599,8 +14601,11 @@
       <c r="C58">
         <v>6</v>
       </c>
-      <c r="G58" s="2" t="s">
-        <v>54</v>
+      <c r="D58">
+        <v>6</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.3">
@@ -14613,8 +14618,11 @@
       <c r="C59">
         <v>5</v>
       </c>
-      <c r="G59" s="14" t="s">
-        <v>55</v>
+      <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.3">
@@ -14625,10 +14633,13 @@
         <v>45003</v>
       </c>
       <c r="C60">
+        <v>5</v>
+      </c>
+      <c r="D60">
         <v>4</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.3">
@@ -14641,6 +14652,12 @@
       <c r="C61">
         <v>4</v>
       </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
@@ -14651,6 +14668,12 @@
       </c>
       <c r="C62">
         <v>3</v>
+      </c>
+      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Locking, Charging up, other special effects
</commit_message>
<xml_diff>
--- a/Burndown.xlsx
+++ b/Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c4e25a7e6f3dc489/Documents/GitHub/ConcurrentProgrammingGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1000" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F00DFBDC-84E1-4FA8-B6B0-5D053FC82FC3}"/>
+  <xr:revisionPtr revIDLastSave="1013" documentId="10_ncr:40000_{8EF4B8C0-E1E8-45DD-99BE-DA8156BBCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57643BAC-E9D6-4277-AB11-358F4F37120D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,12 +281,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,7 +300,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -323,7 +317,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -627,12 +620,6 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2961,18 +2948,6 @@
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4691,19 +4666,19 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
@@ -5646,6 +5621,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13748,8 +13729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z40" sqref="Z40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13894,9 +13875,6 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
       <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
@@ -13910,9 +13888,6 @@
         <v>44966</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -14157,9 +14132,6 @@
       <c r="C28">
         <v>2</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
       <c r="AA28" s="8"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.3">
@@ -14172,9 +14144,6 @@
       <c r="C29">
         <v>2</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
       <c r="AA29" s="8"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.3">
@@ -14187,9 +14156,6 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
       <c r="AA30" s="8"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.3">
@@ -14200,9 +14166,6 @@
         <v>44981</v>
       </c>
       <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
         <v>0</v>
       </c>
       <c r="AA31" s="8"/>
@@ -14347,7 +14310,7 @@
         <v>4</v>
       </c>
       <c r="D40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>35</v>
@@ -14365,7 +14328,7 @@
         <v>4</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AA41" s="8"/>
     </row>
@@ -14380,7 +14343,7 @@
         <v>3</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA42" s="8"/>
     </row>
@@ -14395,7 +14358,7 @@
         <v>3</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA43" s="8"/>
     </row>
@@ -14410,7 +14373,7 @@
         <v>2</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA44" s="8"/>
     </row>
@@ -14587,7 +14550,7 @@
       <c r="D57">
         <v>6</v>
       </c>
-      <c r="G57" s="14" t="s">
+      <c r="G57" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -14604,7 +14567,7 @@
       <c r="D58">
         <v>6</v>
       </c>
-      <c r="G58" s="14" t="s">
+      <c r="G58" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -14686,6 +14649,9 @@
       <c r="C63">
         <v>2</v>
       </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
@@ -14696,6 +14662,9 @@
       </c>
       <c r="C64">
         <v>1</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -14746,23 +14715,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
       <c r="R1" s="10"/>

</xml_diff>